<commit_message>
add 3d prined file
Author: IcyCat
Date: 13/09/22

[MOD]
- add cable holder part
- add camera holder part
</commit_message>
<xml_diff>
--- a/Estimation/CostEstimation.xlsx
+++ b/Estimation/CostEstimation.xlsx
@@ -585,40 +585,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,13 +955,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="23" t="s">
         <v>23</v>
       </c>
@@ -995,7 +995,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
@@ -1022,7 +1022,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="2">
         <v>1.6</v>
       </c>
@@ -1047,7 +1047,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="2">
         <v>1.2</v>
       </c>
@@ -1072,7 +1072,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="2">
         <v>0.3</v>
       </c>
@@ -1224,7 +1224,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="27" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1240,10 +1240,10 @@
         <f>$I$12*C12</f>
         <v>1600</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="34">
+      <c r="I12" s="26">
         <v>16</v>
       </c>
     </row>
@@ -1273,12 +1273,12 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
       <c r="E14" s="18">
         <f>SUM(E3:E13)</f>
         <v>17069</v>
@@ -1286,12 +1286,18 @@
       <c r="F14" s="20"/>
       <c r="G14" s="9"/>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f>SUM(D3:D6)</f>
+        <v>26</v>
+      </c>
+    </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1313,7 +1319,7 @@
       <c r="G17" s="22"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="2">
@@ -1334,7 +1340,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="2">
         <v>0.6</v>
       </c>
@@ -1353,7 +1359,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="2">
         <v>0.75</v>
       </c>
@@ -1372,7 +1378,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="2">
         <v>0.95</v>
       </c>
@@ -1391,7 +1397,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="2">
         <v>0.7</v>
       </c>
@@ -1410,7 +1416,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="2">
         <v>0.3</v>
       </c>
@@ -1528,7 +1534,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="27" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1565,12 +1571,12 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="18">
         <f>SUM(E18:E30)</f>
         <v>17872.599999999999</v>

</xml_diff>